<commit_message>
wijzigingen mbt 2nd projectleider in zowel werkbestand als algemeen overzicht.
</commit_message>
<xml_diff>
--- a/Kolommenmapping per bron.xlsx
+++ b/Kolommenmapping per bron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67E715D-29F4-4137-BD65-398A74A5E0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77487D7-36DC-4B94-AB4F-61980BE42B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
   <si>
     <t>Projectnummer</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Actiepunten Elders</t>
+  </si>
+  <si>
+    <t>2e projectleider</t>
+  </si>
+  <si>
+    <t>2e Projectleider</t>
   </si>
 </sst>
 </file>
@@ -569,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,339 +679,339 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="E13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="5" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="5" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="5" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>49</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -1013,20 +1019,37 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Werkelijk resultaat kolom toegevoegd aan overview. Eveneens wordt deze nu berekend door werkelijke opbrenst - werkelijke kosten = werkelijk resultaat
</commit_message>
<xml_diff>
--- a/Kolommenmapping per bron.xlsx
+++ b/Kolommenmapping per bron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77487D7-36DC-4B94-AB4F-61980BE42B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5626392D-303B-430C-AE62-D9D9D20B4B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
   <si>
     <t>Projectnummer</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>2e Projectleider</t>
+  </si>
+  <si>
+    <t>Werkelijk resultaat</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,167 +871,167 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="5" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="5" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="5" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="5" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="5"/>
+      <c r="G22" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>49</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="5"/>
+      <c r="G24" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1036,20 +1039,37 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
deleted emoijs for sync.py to work. Also various changes to make overview for projects to be closed (not done yet)
</commit_message>
<xml_diff>
--- a/Kolommenmapping per bron.xlsx
+++ b/Kolommenmapping per bron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5626392D-303B-430C-AE62-D9D9D20B4B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C21D8-7F19-4167-9C0D-4327BC1EE97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>Projectnummer</t>
   </si>
@@ -581,7 +581,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,7 +816,9 @@
         <v>35</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">

</xml_diff>

<commit_message>
sluiten toegevoegd als bevestiging van projectlieders dat iets gesloten kan worden
</commit_message>
<xml_diff>
--- a/Kolommenmapping per bron.xlsx
+++ b/Kolommenmapping per bron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A915180-C95B-4B0E-A237-6B4D02F313B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6212EA-CCA9-48CF-B60E-197954C3CA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
   <si>
     <t>Projectnummer</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Informatie</t>
+  </si>
+  <si>
+    <t>Sluiten</t>
   </si>
 </sst>
 </file>
@@ -307,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -318,8 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -600,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,116 +994,116 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="5" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="5"/>
+      <c r="G25" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>49</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>46</v>
+      <c r="C28" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -1110,62 +1111,64 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>47</v>
+      <c r="C29" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>53</v>
+      <c r="A30" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="B31" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>57</v>
+      <c r="C31" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="5"/>
+      <c r="G31" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>58</v>
+      <c r="A32" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>58</v>
+      <c r="C32" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1173,14 +1176,14 @@
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>59</v>
+      <c r="A33" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>59</v>
+      <c r="C33" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -1188,14 +1191,14 @@
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>60</v>
+      <c r="A34" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B34" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>60</v>
+      <c r="C34" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1203,20 +1206,35 @@
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>61</v>
+      <c r="A35" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B35" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>61</v>
+      <c r="C35" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="5"/>
     </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tier 1 summary in werkbestand to close projects
</commit_message>
<xml_diff>
--- a/Kolommenmapping per bron.xlsx
+++ b/Kolommenmapping per bron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6212EA-CCA9-48CF-B60E-197954C3CA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319FDC2E-9125-4CB0-91D8-BF8E1A463371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>